<commit_message>
chg: Prep for D2.1: JFC D&G, VID INTSUM from D1 published. Weather information for D2.1 published.
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/AUTHENTICATION TABLE.xlsx
+++ b/MISSION INFORMATION/AUTHENTICATION TABLE.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="20730" windowHeight="11760" activeTab="2"/>
@@ -1297,8 +1297,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1306,25 +1309,25 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1342,52 +1345,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1409,6 +1373,42 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2099,44 +2099,44 @@
   <sheetData>
     <row r="1" spans="1:80" ht="46.5">
       <c r="A1" s="29"/>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="76"/>
-      <c r="U1" s="76"/>
-      <c r="V1" s="76"/>
-      <c r="W1" s="76"/>
-      <c r="X1" s="76"/>
-      <c r="Y1" s="76"/>
-      <c r="Z1" s="76"/>
-      <c r="AA1" s="76"/>
-      <c r="AB1" s="76"/>
-      <c r="AC1" s="76"/>
-      <c r="AD1" s="76"/>
-      <c r="AE1" s="76"/>
-      <c r="AF1" s="76"/>
-      <c r="AG1" s="76"/>
-      <c r="AH1" s="76"/>
-      <c r="AI1" s="76"/>
-      <c r="AJ1" s="76"/>
-      <c r="AK1" s="76"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="77"/>
+      <c r="AD1" s="77"/>
+      <c r="AE1" s="77"/>
+      <c r="AF1" s="77"/>
+      <c r="AG1" s="77"/>
+      <c r="AH1" s="77"/>
+      <c r="AI1" s="77"/>
+      <c r="AJ1" s="77"/>
+      <c r="AK1" s="77"/>
       <c r="AL1" s="30"/>
     </row>
     <row r="2" spans="1:80" ht="26.25">
@@ -2167,18 +2167,18 @@
       <c r="Y2" s="33"/>
       <c r="Z2" s="33"/>
       <c r="AA2" s="33"/>
-      <c r="AB2" s="77" t="s">
+      <c r="AB2" s="78" t="s">
         <v>243</v>
       </c>
-      <c r="AC2" s="77"/>
-      <c r="AD2" s="77"/>
-      <c r="AE2" s="77"/>
-      <c r="AF2" s="77"/>
-      <c r="AG2" s="77"/>
-      <c r="AH2" s="77"/>
-      <c r="AI2" s="77"/>
-      <c r="AJ2" s="77"/>
-      <c r="AK2" s="77"/>
+      <c r="AC2" s="78"/>
+      <c r="AD2" s="78"/>
+      <c r="AE2" s="78"/>
+      <c r="AF2" s="78"/>
+      <c r="AG2" s="78"/>
+      <c r="AH2" s="78"/>
+      <c r="AI2" s="78"/>
+      <c r="AJ2" s="78"/>
+      <c r="AK2" s="78"/>
       <c r="AL2" s="34"/>
     </row>
     <row r="3" spans="1:80" ht="23.25">
@@ -3102,99 +3102,99 @@
     <row r="11" spans="1:80" ht="23.25">
       <c r="A11" s="31"/>
       <c r="B11" s="40"/>
-      <c r="C11" s="78">
+      <c r="C11" s="75">
         <v>5</v>
       </c>
-      <c r="D11" s="78"/>
-      <c r="E11" s="78"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
       <c r="F11" s="40"/>
-      <c r="G11" s="78">
+      <c r="G11" s="75">
         <v>7</v>
       </c>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="75"/>
       <c r="J11" s="40"/>
-      <c r="K11" s="78">
+      <c r="K11" s="75">
         <v>2</v>
       </c>
-      <c r="L11" s="78"/>
+      <c r="L11" s="75"/>
       <c r="M11" s="40"/>
-      <c r="N11" s="78">
+      <c r="N11" s="75">
         <v>3</v>
       </c>
-      <c r="O11" s="78"/>
+      <c r="O11" s="75"/>
       <c r="P11" s="40"/>
-      <c r="Q11" s="78">
+      <c r="Q11" s="75">
         <v>4</v>
       </c>
-      <c r="R11" s="78"/>
+      <c r="R11" s="75"/>
       <c r="S11" s="40"/>
-      <c r="T11" s="78">
+      <c r="T11" s="75">
         <v>1</v>
       </c>
-      <c r="U11" s="78"/>
-      <c r="V11" s="78"/>
+      <c r="U11" s="75"/>
+      <c r="V11" s="75"/>
       <c r="W11" s="40"/>
-      <c r="X11" s="78">
+      <c r="X11" s="75">
         <v>6</v>
       </c>
-      <c r="Y11" s="78"/>
-      <c r="Z11" s="78"/>
+      <c r="Y11" s="75"/>
+      <c r="Z11" s="75"/>
       <c r="AA11" s="40"/>
-      <c r="AB11" s="78">
+      <c r="AB11" s="75">
         <v>0</v>
       </c>
-      <c r="AC11" s="78"/>
-      <c r="AD11" s="78"/>
+      <c r="AC11" s="75"/>
+      <c r="AD11" s="75"/>
       <c r="AE11" s="40"/>
-      <c r="AF11" s="78">
+      <c r="AF11" s="75">
         <v>8</v>
       </c>
-      <c r="AG11" s="78"/>
+      <c r="AG11" s="75"/>
       <c r="AH11" s="40"/>
-      <c r="AI11" s="78">
+      <c r="AI11" s="75">
         <v>9</v>
       </c>
-      <c r="AJ11" s="78"/>
-      <c r="AK11" s="78"/>
+      <c r="AJ11" s="75"/>
+      <c r="AK11" s="75"/>
       <c r="AL11" s="41"/>
-      <c r="AR11" s="75"/>
-      <c r="AS11" s="75"/>
-      <c r="AT11" s="75"/>
-      <c r="AU11" s="75"/>
-      <c r="AV11" s="75"/>
+      <c r="AR11" s="79"/>
+      <c r="AS11" s="79"/>
+      <c r="AT11" s="79"/>
+      <c r="AU11" s="79"/>
+      <c r="AV11" s="79"/>
       <c r="AW11" s="74"/>
-      <c r="AX11" s="75"/>
-      <c r="AY11" s="75"/>
-      <c r="AZ11" s="75"/>
+      <c r="AX11" s="79"/>
+      <c r="AY11" s="79"/>
+      <c r="AZ11" s="79"/>
       <c r="BA11" s="74"/>
-      <c r="BB11" s="75"/>
-      <c r="BC11" s="75"/>
+      <c r="BB11" s="79"/>
+      <c r="BC11" s="79"/>
       <c r="BD11" s="74"/>
-      <c r="BE11" s="75"/>
-      <c r="BF11" s="75"/>
+      <c r="BE11" s="79"/>
+      <c r="BF11" s="79"/>
       <c r="BG11" s="74"/>
-      <c r="BH11" s="75"/>
-      <c r="BI11" s="75"/>
+      <c r="BH11" s="79"/>
+      <c r="BI11" s="79"/>
       <c r="BJ11" s="74"/>
-      <c r="BK11" s="75"/>
-      <c r="BL11" s="75"/>
-      <c r="BM11" s="75"/>
+      <c r="BK11" s="79"/>
+      <c r="BL11" s="79"/>
+      <c r="BM11" s="79"/>
       <c r="BN11" s="74"/>
-      <c r="BO11" s="75"/>
-      <c r="BP11" s="75"/>
-      <c r="BQ11" s="75"/>
+      <c r="BO11" s="79"/>
+      <c r="BP11" s="79"/>
+      <c r="BQ11" s="79"/>
       <c r="BR11" s="74"/>
-      <c r="BS11" s="75"/>
-      <c r="BT11" s="75"/>
-      <c r="BU11" s="75"/>
+      <c r="BS11" s="79"/>
+      <c r="BT11" s="79"/>
+      <c r="BU11" s="79"/>
       <c r="BV11" s="74"/>
-      <c r="BW11" s="75"/>
-      <c r="BX11" s="75"/>
+      <c r="BW11" s="79"/>
+      <c r="BX11" s="79"/>
       <c r="BY11" s="74"/>
-      <c r="BZ11" s="75"/>
-      <c r="CA11" s="75"/>
-      <c r="CB11" s="75"/>
+      <c r="BZ11" s="79"/>
+      <c r="CA11" s="79"/>
+      <c r="CB11" s="79"/>
     </row>
     <row r="12" spans="1:80" ht="23.25">
       <c r="A12" s="31"/>
@@ -3985,99 +3985,99 @@
     <row r="18" spans="1:80" ht="23.25">
       <c r="A18" s="31"/>
       <c r="B18" s="36"/>
-      <c r="C18" s="78">
+      <c r="C18" s="75">
         <v>5</v>
       </c>
-      <c r="D18" s="78"/>
-      <c r="E18" s="78"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="75"/>
       <c r="F18" s="40"/>
-      <c r="G18" s="78">
+      <c r="G18" s="75">
         <v>7</v>
       </c>
-      <c r="H18" s="78"/>
-      <c r="I18" s="78"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="75"/>
       <c r="J18" s="40"/>
-      <c r="K18" s="78">
+      <c r="K18" s="75">
         <v>2</v>
       </c>
-      <c r="L18" s="78"/>
+      <c r="L18" s="75"/>
       <c r="M18" s="40"/>
-      <c r="N18" s="78">
+      <c r="N18" s="75">
         <v>3</v>
       </c>
-      <c r="O18" s="78"/>
+      <c r="O18" s="75"/>
       <c r="P18" s="40"/>
-      <c r="Q18" s="78">
+      <c r="Q18" s="75">
         <v>4</v>
       </c>
-      <c r="R18" s="78"/>
+      <c r="R18" s="75"/>
       <c r="S18" s="40"/>
-      <c r="T18" s="78">
+      <c r="T18" s="75">
         <v>1</v>
       </c>
-      <c r="U18" s="78"/>
-      <c r="V18" s="78"/>
+      <c r="U18" s="75"/>
+      <c r="V18" s="75"/>
       <c r="W18" s="40"/>
-      <c r="X18" s="78">
+      <c r="X18" s="75">
         <v>6</v>
       </c>
-      <c r="Y18" s="78"/>
-      <c r="Z18" s="78"/>
+      <c r="Y18" s="75"/>
+      <c r="Z18" s="75"/>
       <c r="AA18" s="40"/>
-      <c r="AB18" s="78">
+      <c r="AB18" s="75">
         <v>0</v>
       </c>
-      <c r="AC18" s="78"/>
-      <c r="AD18" s="78"/>
+      <c r="AC18" s="75"/>
+      <c r="AD18" s="75"/>
       <c r="AE18" s="40"/>
-      <c r="AF18" s="78">
+      <c r="AF18" s="75">
         <v>8</v>
       </c>
-      <c r="AG18" s="78"/>
+      <c r="AG18" s="75"/>
       <c r="AH18" s="40"/>
-      <c r="AI18" s="78">
+      <c r="AI18" s="75">
         <v>9</v>
       </c>
-      <c r="AJ18" s="78"/>
-      <c r="AK18" s="78"/>
+      <c r="AJ18" s="75"/>
+      <c r="AK18" s="75"/>
       <c r="AL18" s="41"/>
-      <c r="AR18" s="75"/>
-      <c r="AS18" s="75"/>
-      <c r="AT18" s="75"/>
-      <c r="AU18" s="75"/>
-      <c r="AV18" s="75"/>
+      <c r="AR18" s="79"/>
+      <c r="AS18" s="79"/>
+      <c r="AT18" s="79"/>
+      <c r="AU18" s="79"/>
+      <c r="AV18" s="79"/>
       <c r="AW18" s="74"/>
-      <c r="AX18" s="75"/>
-      <c r="AY18" s="75"/>
-      <c r="AZ18" s="75"/>
+      <c r="AX18" s="79"/>
+      <c r="AY18" s="79"/>
+      <c r="AZ18" s="79"/>
       <c r="BA18" s="74"/>
-      <c r="BB18" s="75"/>
-      <c r="BC18" s="75"/>
+      <c r="BB18" s="79"/>
+      <c r="BC18" s="79"/>
       <c r="BD18" s="74"/>
-      <c r="BE18" s="75"/>
-      <c r="BF18" s="75"/>
+      <c r="BE18" s="79"/>
+      <c r="BF18" s="79"/>
       <c r="BG18" s="74"/>
-      <c r="BH18" s="75"/>
-      <c r="BI18" s="75"/>
+      <c r="BH18" s="79"/>
+      <c r="BI18" s="79"/>
       <c r="BJ18" s="74"/>
-      <c r="BK18" s="75"/>
-      <c r="BL18" s="75"/>
-      <c r="BM18" s="75"/>
+      <c r="BK18" s="79"/>
+      <c r="BL18" s="79"/>
+      <c r="BM18" s="79"/>
       <c r="BN18" s="74"/>
-      <c r="BO18" s="75"/>
-      <c r="BP18" s="75"/>
-      <c r="BQ18" s="75"/>
+      <c r="BO18" s="79"/>
+      <c r="BP18" s="79"/>
+      <c r="BQ18" s="79"/>
       <c r="BR18" s="74"/>
-      <c r="BS18" s="75"/>
-      <c r="BT18" s="75"/>
-      <c r="BU18" s="75"/>
+      <c r="BS18" s="79"/>
+      <c r="BT18" s="79"/>
+      <c r="BU18" s="79"/>
       <c r="BV18" s="74"/>
-      <c r="BW18" s="75"/>
-      <c r="BX18" s="75"/>
+      <c r="BW18" s="79"/>
+      <c r="BX18" s="79"/>
       <c r="BY18" s="74"/>
-      <c r="BZ18" s="75"/>
-      <c r="CA18" s="75"/>
-      <c r="CB18" s="75"/>
+      <c r="BZ18" s="79"/>
+      <c r="CA18" s="79"/>
+      <c r="CB18" s="79"/>
     </row>
     <row r="19" spans="1:80" ht="23.25">
       <c r="A19" s="31"/>
@@ -4868,99 +4868,99 @@
     <row r="25" spans="1:80" ht="23.25">
       <c r="A25" s="31"/>
       <c r="B25" s="36"/>
-      <c r="C25" s="78">
+      <c r="C25" s="75">
         <v>5</v>
       </c>
-      <c r="D25" s="78"/>
-      <c r="E25" s="78"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
       <c r="F25" s="40"/>
-      <c r="G25" s="78">
+      <c r="G25" s="75">
         <v>7</v>
       </c>
-      <c r="H25" s="78"/>
-      <c r="I25" s="78"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="75"/>
       <c r="J25" s="40"/>
-      <c r="K25" s="78">
+      <c r="K25" s="75">
         <v>2</v>
       </c>
-      <c r="L25" s="78"/>
+      <c r="L25" s="75"/>
       <c r="M25" s="40"/>
-      <c r="N25" s="78">
+      <c r="N25" s="75">
         <v>3</v>
       </c>
-      <c r="O25" s="78"/>
+      <c r="O25" s="75"/>
       <c r="P25" s="40"/>
-      <c r="Q25" s="78">
+      <c r="Q25" s="75">
         <v>4</v>
       </c>
-      <c r="R25" s="78"/>
+      <c r="R25" s="75"/>
       <c r="S25" s="40"/>
-      <c r="T25" s="78">
+      <c r="T25" s="75">
         <v>1</v>
       </c>
-      <c r="U25" s="78"/>
-      <c r="V25" s="78"/>
+      <c r="U25" s="75"/>
+      <c r="V25" s="75"/>
       <c r="W25" s="40"/>
-      <c r="X25" s="78">
+      <c r="X25" s="75">
         <v>6</v>
       </c>
-      <c r="Y25" s="78"/>
-      <c r="Z25" s="78"/>
+      <c r="Y25" s="75"/>
+      <c r="Z25" s="75"/>
       <c r="AA25" s="40"/>
-      <c r="AB25" s="78">
+      <c r="AB25" s="75">
         <v>0</v>
       </c>
-      <c r="AC25" s="78"/>
-      <c r="AD25" s="78"/>
+      <c r="AC25" s="75"/>
+      <c r="AD25" s="75"/>
       <c r="AE25" s="40"/>
-      <c r="AF25" s="78">
+      <c r="AF25" s="75">
         <v>8</v>
       </c>
-      <c r="AG25" s="78"/>
+      <c r="AG25" s="75"/>
       <c r="AH25" s="40"/>
-      <c r="AI25" s="78">
+      <c r="AI25" s="75">
         <v>9</v>
       </c>
-      <c r="AJ25" s="78"/>
-      <c r="AK25" s="78"/>
+      <c r="AJ25" s="75"/>
+      <c r="AK25" s="75"/>
       <c r="AL25" s="41"/>
-      <c r="AR25" s="75"/>
-      <c r="AS25" s="75"/>
-      <c r="AT25" s="75"/>
-      <c r="AU25" s="75"/>
-      <c r="AV25" s="75"/>
+      <c r="AR25" s="79"/>
+      <c r="AS25" s="79"/>
+      <c r="AT25" s="79"/>
+      <c r="AU25" s="79"/>
+      <c r="AV25" s="79"/>
       <c r="AW25" s="74"/>
-      <c r="AX25" s="75"/>
-      <c r="AY25" s="75"/>
-      <c r="AZ25" s="75"/>
+      <c r="AX25" s="79"/>
+      <c r="AY25" s="79"/>
+      <c r="AZ25" s="79"/>
       <c r="BA25" s="74"/>
-      <c r="BB25" s="75"/>
-      <c r="BC25" s="75"/>
+      <c r="BB25" s="79"/>
+      <c r="BC25" s="79"/>
       <c r="BD25" s="74"/>
-      <c r="BE25" s="75"/>
-      <c r="BF25" s="75"/>
+      <c r="BE25" s="79"/>
+      <c r="BF25" s="79"/>
       <c r="BG25" s="74"/>
-      <c r="BH25" s="75"/>
-      <c r="BI25" s="75"/>
+      <c r="BH25" s="79"/>
+      <c r="BI25" s="79"/>
       <c r="BJ25" s="74"/>
-      <c r="BK25" s="75"/>
-      <c r="BL25" s="75"/>
-      <c r="BM25" s="75"/>
+      <c r="BK25" s="79"/>
+      <c r="BL25" s="79"/>
+      <c r="BM25" s="79"/>
       <c r="BN25" s="74"/>
-      <c r="BO25" s="75"/>
-      <c r="BP25" s="75"/>
-      <c r="BQ25" s="75"/>
+      <c r="BO25" s="79"/>
+      <c r="BP25" s="79"/>
+      <c r="BQ25" s="79"/>
       <c r="BR25" s="74"/>
-      <c r="BS25" s="75"/>
-      <c r="BT25" s="75"/>
-      <c r="BU25" s="75"/>
+      <c r="BS25" s="79"/>
+      <c r="BT25" s="79"/>
+      <c r="BU25" s="79"/>
       <c r="BV25" s="74"/>
-      <c r="BW25" s="75"/>
-      <c r="BX25" s="75"/>
+      <c r="BW25" s="79"/>
+      <c r="BX25" s="79"/>
       <c r="BY25" s="74"/>
-      <c r="BZ25" s="75"/>
-      <c r="CA25" s="75"/>
-      <c r="CB25" s="75"/>
+      <c r="BZ25" s="79"/>
+      <c r="CA25" s="79"/>
+      <c r="CB25" s="79"/>
     </row>
     <row r="26" spans="1:80" ht="23.25">
       <c r="A26" s="31"/>
@@ -5976,103 +5976,103 @@
     <row r="34" spans="1:38" ht="23.25">
       <c r="A34" s="31"/>
       <c r="B34" s="42"/>
-      <c r="C34" s="78">
+      <c r="C34" s="75">
         <v>0</v>
       </c>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="75"/>
       <c r="F34" s="40"/>
-      <c r="G34" s="78">
+      <c r="G34" s="75">
         <v>1</v>
       </c>
-      <c r="H34" s="78"/>
-      <c r="I34" s="78"/>
+      <c r="H34" s="75"/>
+      <c r="I34" s="75"/>
       <c r="J34" s="40"/>
-      <c r="K34" s="78">
+      <c r="K34" s="75">
         <v>2</v>
       </c>
-      <c r="L34" s="78"/>
+      <c r="L34" s="75"/>
       <c r="M34" s="40"/>
-      <c r="N34" s="78">
+      <c r="N34" s="75">
         <v>3</v>
       </c>
-      <c r="O34" s="78"/>
+      <c r="O34" s="75"/>
       <c r="P34" s="40"/>
-      <c r="Q34" s="78">
+      <c r="Q34" s="75">
         <v>4</v>
       </c>
-      <c r="R34" s="78"/>
+      <c r="R34" s="75"/>
       <c r="S34" s="40"/>
-      <c r="T34" s="78">
+      <c r="T34" s="75">
         <v>5</v>
       </c>
-      <c r="U34" s="78"/>
-      <c r="V34" s="78"/>
+      <c r="U34" s="75"/>
+      <c r="V34" s="75"/>
       <c r="W34" s="40"/>
-      <c r="X34" s="78">
+      <c r="X34" s="75">
         <v>6</v>
       </c>
-      <c r="Y34" s="78"/>
-      <c r="Z34" s="78"/>
+      <c r="Y34" s="75"/>
+      <c r="Z34" s="75"/>
       <c r="AA34" s="40"/>
-      <c r="AB34" s="78">
+      <c r="AB34" s="75">
         <v>7</v>
       </c>
-      <c r="AC34" s="78"/>
-      <c r="AD34" s="78"/>
+      <c r="AC34" s="75"/>
+      <c r="AD34" s="75"/>
       <c r="AE34" s="40"/>
-      <c r="AF34" s="78">
+      <c r="AF34" s="75">
         <v>8</v>
       </c>
-      <c r="AG34" s="78"/>
+      <c r="AG34" s="75"/>
       <c r="AH34" s="40"/>
-      <c r="AI34" s="78">
+      <c r="AI34" s="75">
         <v>9</v>
       </c>
-      <c r="AJ34" s="78"/>
-      <c r="AK34" s="78"/>
+      <c r="AJ34" s="75"/>
+      <c r="AK34" s="75"/>
       <c r="AL34" s="41"/>
     </row>
     <row r="35" spans="1:38" ht="26.25">
       <c r="A35" s="31"/>
-      <c r="B35" s="79" t="s">
+      <c r="B35" s="76" t="s">
         <v>244</v>
       </c>
-      <c r="C35" s="79"/>
-      <c r="D35" s="79"/>
-      <c r="E35" s="79"/>
-      <c r="F35" s="79"/>
-      <c r="G35" s="79"/>
-      <c r="H35" s="79"/>
-      <c r="I35" s="79"/>
-      <c r="J35" s="79"/>
-      <c r="K35" s="79"/>
-      <c r="L35" s="79"/>
-      <c r="M35" s="79"/>
-      <c r="N35" s="79"/>
-      <c r="O35" s="79"/>
-      <c r="P35" s="79"/>
-      <c r="Q35" s="79"/>
-      <c r="R35" s="79"/>
-      <c r="S35" s="79"/>
-      <c r="T35" s="79"/>
-      <c r="U35" s="79"/>
-      <c r="V35" s="79"/>
-      <c r="W35" s="79"/>
-      <c r="X35" s="79"/>
-      <c r="Y35" s="79"/>
-      <c r="Z35" s="79"/>
-      <c r="AA35" s="79"/>
-      <c r="AB35" s="79"/>
-      <c r="AC35" s="79"/>
-      <c r="AD35" s="79"/>
-      <c r="AE35" s="79"/>
-      <c r="AF35" s="79"/>
-      <c r="AG35" s="79"/>
-      <c r="AH35" s="79"/>
-      <c r="AI35" s="79"/>
-      <c r="AJ35" s="79"/>
-      <c r="AK35" s="79"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="76"/>
+      <c r="E35" s="76"/>
+      <c r="F35" s="76"/>
+      <c r="G35" s="76"/>
+      <c r="H35" s="76"/>
+      <c r="I35" s="76"/>
+      <c r="J35" s="76"/>
+      <c r="K35" s="76"/>
+      <c r="L35" s="76"/>
+      <c r="M35" s="76"/>
+      <c r="N35" s="76"/>
+      <c r="O35" s="76"/>
+      <c r="P35" s="76"/>
+      <c r="Q35" s="76"/>
+      <c r="R35" s="76"/>
+      <c r="S35" s="76"/>
+      <c r="T35" s="76"/>
+      <c r="U35" s="76"/>
+      <c r="V35" s="76"/>
+      <c r="W35" s="76"/>
+      <c r="X35" s="76"/>
+      <c r="Y35" s="76"/>
+      <c r="Z35" s="76"/>
+      <c r="AA35" s="76"/>
+      <c r="AB35" s="76"/>
+      <c r="AC35" s="76"/>
+      <c r="AD35" s="76"/>
+      <c r="AE35" s="76"/>
+      <c r="AF35" s="76"/>
+      <c r="AG35" s="76"/>
+      <c r="AH35" s="76"/>
+      <c r="AI35" s="76"/>
+      <c r="AJ35" s="76"/>
+      <c r="AK35" s="76"/>
       <c r="AL35" s="43"/>
     </row>
     <row r="36" spans="1:38">
@@ -6277,6 +6277,66 @@
     </row>
   </sheetData>
   <mergeCells count="76">
+    <mergeCell ref="BZ25:CB25"/>
+    <mergeCell ref="BH25:BI25"/>
+    <mergeCell ref="BK25:BM25"/>
+    <mergeCell ref="BO25:BQ25"/>
+    <mergeCell ref="BS25:BU25"/>
+    <mergeCell ref="BW25:BX25"/>
+    <mergeCell ref="AR25:AS25"/>
+    <mergeCell ref="AT25:AV25"/>
+    <mergeCell ref="AX25:AZ25"/>
+    <mergeCell ref="BB25:BC25"/>
+    <mergeCell ref="BE25:BF25"/>
+    <mergeCell ref="BZ11:CB11"/>
+    <mergeCell ref="AR18:AS18"/>
+    <mergeCell ref="AT18:AV18"/>
+    <mergeCell ref="AX18:AZ18"/>
+    <mergeCell ref="BB18:BC18"/>
+    <mergeCell ref="BE18:BF18"/>
+    <mergeCell ref="BH18:BI18"/>
+    <mergeCell ref="BK18:BM18"/>
+    <mergeCell ref="BO18:BQ18"/>
+    <mergeCell ref="BS18:BU18"/>
+    <mergeCell ref="BW18:BX18"/>
+    <mergeCell ref="BZ18:CB18"/>
+    <mergeCell ref="BH11:BI11"/>
+    <mergeCell ref="BK11:BM11"/>
+    <mergeCell ref="BO11:BQ11"/>
+    <mergeCell ref="BS11:BU11"/>
+    <mergeCell ref="BW11:BX11"/>
+    <mergeCell ref="AR11:AS11"/>
+    <mergeCell ref="AT11:AV11"/>
+    <mergeCell ref="AX11:AZ11"/>
+    <mergeCell ref="BB11:BC11"/>
+    <mergeCell ref="BE11:BF11"/>
+    <mergeCell ref="B1:AK1"/>
+    <mergeCell ref="AB2:AK2"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="T11:V11"/>
+    <mergeCell ref="X11:Z11"/>
+    <mergeCell ref="AB11:AD11"/>
+    <mergeCell ref="AF11:AG11"/>
+    <mergeCell ref="AI11:AK11"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="T18:V18"/>
+    <mergeCell ref="X18:Z18"/>
+    <mergeCell ref="AB18:AD18"/>
+    <mergeCell ref="AF18:AG18"/>
+    <mergeCell ref="AI18:AK18"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="Q25:R25"/>
     <mergeCell ref="T25:V25"/>
     <mergeCell ref="B35:AK35"/>
     <mergeCell ref="X25:Z25"/>
@@ -6293,66 +6353,6 @@
     <mergeCell ref="AB34:AD34"/>
     <mergeCell ref="AF34:AG34"/>
     <mergeCell ref="AI34:AK34"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="T18:V18"/>
-    <mergeCell ref="X18:Z18"/>
-    <mergeCell ref="AB18:AD18"/>
-    <mergeCell ref="AF18:AG18"/>
-    <mergeCell ref="AI18:AK18"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="B1:AK1"/>
-    <mergeCell ref="AB2:AK2"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="T11:V11"/>
-    <mergeCell ref="X11:Z11"/>
-    <mergeCell ref="AB11:AD11"/>
-    <mergeCell ref="AF11:AG11"/>
-    <mergeCell ref="AI11:AK11"/>
-    <mergeCell ref="BW11:BX11"/>
-    <mergeCell ref="AR11:AS11"/>
-    <mergeCell ref="AT11:AV11"/>
-    <mergeCell ref="AX11:AZ11"/>
-    <mergeCell ref="BB11:BC11"/>
-    <mergeCell ref="BE11:BF11"/>
-    <mergeCell ref="BZ11:CB11"/>
-    <mergeCell ref="AR18:AS18"/>
-    <mergeCell ref="AT18:AV18"/>
-    <mergeCell ref="AX18:AZ18"/>
-    <mergeCell ref="BB18:BC18"/>
-    <mergeCell ref="BE18:BF18"/>
-    <mergeCell ref="BH18:BI18"/>
-    <mergeCell ref="BK18:BM18"/>
-    <mergeCell ref="BO18:BQ18"/>
-    <mergeCell ref="BS18:BU18"/>
-    <mergeCell ref="BW18:BX18"/>
-    <mergeCell ref="BZ18:CB18"/>
-    <mergeCell ref="BH11:BI11"/>
-    <mergeCell ref="BK11:BM11"/>
-    <mergeCell ref="BO11:BQ11"/>
-    <mergeCell ref="BS11:BU11"/>
-    <mergeCell ref="AR25:AS25"/>
-    <mergeCell ref="AT25:AV25"/>
-    <mergeCell ref="AX25:AZ25"/>
-    <mergeCell ref="BB25:BC25"/>
-    <mergeCell ref="BE25:BF25"/>
-    <mergeCell ref="BZ25:CB25"/>
-    <mergeCell ref="BH25:BI25"/>
-    <mergeCell ref="BK25:BM25"/>
-    <mergeCell ref="BO25:BQ25"/>
-    <mergeCell ref="BS25:BU25"/>
-    <mergeCell ref="BW25:BX25"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -6364,7 +6364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AL43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="AL6" sqref="AL6"/>
     </sheetView>
   </sheetViews>
@@ -6393,44 +6393,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="21">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="86"/>
-      <c r="R1" s="86"/>
-      <c r="S1" s="86"/>
-      <c r="T1" s="86"/>
-      <c r="U1" s="86"/>
-      <c r="V1" s="86"/>
-      <c r="W1" s="86"/>
-      <c r="X1" s="86"/>
-      <c r="Y1" s="86"/>
-      <c r="Z1" s="86"/>
-      <c r="AA1" s="86"/>
-      <c r="AB1" s="86"/>
-      <c r="AC1" s="86"/>
-      <c r="AD1" s="86"/>
-      <c r="AE1" s="86"/>
-      <c r="AF1" s="86"/>
-      <c r="AG1" s="86"/>
-      <c r="AH1" s="86"/>
-      <c r="AI1" s="86"/>
-      <c r="AJ1" s="87"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="87"/>
+      <c r="S1" s="87"/>
+      <c r="T1" s="87"/>
+      <c r="U1" s="87"/>
+      <c r="V1" s="87"/>
+      <c r="W1" s="87"/>
+      <c r="X1" s="87"/>
+      <c r="Y1" s="87"/>
+      <c r="Z1" s="87"/>
+      <c r="AA1" s="87"/>
+      <c r="AB1" s="87"/>
+      <c r="AC1" s="87"/>
+      <c r="AD1" s="87"/>
+      <c r="AE1" s="87"/>
+      <c r="AF1" s="87"/>
+      <c r="AG1" s="87"/>
+      <c r="AH1" s="87"/>
+      <c r="AI1" s="87"/>
+      <c r="AJ1" s="88"/>
     </row>
     <row r="2" spans="1:38" ht="15.75">
       <c r="A2" s="4" t="s">
@@ -6461,18 +6461,18 @@
       <c r="X2" s="16"/>
       <c r="Y2" s="16"/>
       <c r="Z2" s="16"/>
-      <c r="AA2" s="88" t="s">
+      <c r="AA2" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="AB2" s="88"/>
-      <c r="AC2" s="88"/>
-      <c r="AD2" s="88"/>
-      <c r="AE2" s="88"/>
-      <c r="AF2" s="88"/>
-      <c r="AG2" s="88"/>
-      <c r="AH2" s="88"/>
-      <c r="AI2" s="88"/>
-      <c r="AJ2" s="89"/>
+      <c r="AB2" s="89"/>
+      <c r="AC2" s="89"/>
+      <c r="AD2" s="89"/>
+      <c r="AE2" s="89"/>
+      <c r="AF2" s="89"/>
+      <c r="AG2" s="89"/>
+      <c r="AH2" s="89"/>
+      <c r="AI2" s="89"/>
+      <c r="AJ2" s="90"/>
     </row>
     <row r="3" spans="1:38" ht="15.75">
       <c r="A3" s="8"/>
@@ -7213,7 +7213,7 @@
         <v>9</v>
       </c>
       <c r="AI11" s="80"/>
-      <c r="AJ11" s="81"/>
+      <c r="AJ11" s="85"/>
     </row>
     <row r="12" spans="1:38" ht="9.9499999999999993" customHeight="1">
       <c r="A12" s="20" t="s">
@@ -7824,7 +7824,7 @@
         <v>9</v>
       </c>
       <c r="AI18" s="80"/>
-      <c r="AJ18" s="81"/>
+      <c r="AJ18" s="85"/>
     </row>
     <row r="19" spans="1:37" ht="9.9499999999999993" customHeight="1">
       <c r="A19" s="10" t="s">
@@ -8434,7 +8434,7 @@
         <v>9</v>
       </c>
       <c r="AI25" s="80"/>
-      <c r="AJ25" s="81"/>
+      <c r="AJ25" s="85"/>
     </row>
     <row r="26" spans="1:37" ht="9.9499999999999993" customHeight="1">
       <c r="A26" s="10" t="s">
@@ -9136,163 +9136,163 @@
         <v>9</v>
       </c>
       <c r="AI33" s="80"/>
-      <c r="AJ33" s="81"/>
+      <c r="AJ33" s="85"/>
     </row>
     <row r="34" spans="1:36">
-      <c r="A34" s="82" t="s">
+      <c r="A34" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="83"/>
-      <c r="C34" s="83"/>
-      <c r="D34" s="83"/>
-      <c r="E34" s="83"/>
-      <c r="F34" s="83"/>
-      <c r="G34" s="83"/>
-      <c r="H34" s="83"/>
-      <c r="I34" s="83"/>
-      <c r="J34" s="83"/>
-      <c r="K34" s="83"/>
-      <c r="L34" s="83"/>
-      <c r="M34" s="83"/>
-      <c r="N34" s="83"/>
-      <c r="O34" s="83"/>
-      <c r="P34" s="83"/>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="83"/>
-      <c r="S34" s="83"/>
-      <c r="T34" s="83"/>
-      <c r="U34" s="83"/>
-      <c r="V34" s="83"/>
-      <c r="W34" s="83"/>
-      <c r="X34" s="83"/>
-      <c r="Y34" s="83"/>
-      <c r="Z34" s="83"/>
-      <c r="AA34" s="83"/>
-      <c r="AB34" s="83"/>
-      <c r="AC34" s="83"/>
-      <c r="AD34" s="83"/>
-      <c r="AE34" s="83"/>
-      <c r="AF34" s="83"/>
-      <c r="AG34" s="83"/>
-      <c r="AH34" s="83"/>
-      <c r="AI34" s="83"/>
-      <c r="AJ34" s="84"/>
+      <c r="B34" s="92"/>
+      <c r="C34" s="92"/>
+      <c r="D34" s="92"/>
+      <c r="E34" s="92"/>
+      <c r="F34" s="92"/>
+      <c r="G34" s="92"/>
+      <c r="H34" s="92"/>
+      <c r="I34" s="92"/>
+      <c r="J34" s="92"/>
+      <c r="K34" s="92"/>
+      <c r="L34" s="92"/>
+      <c r="M34" s="92"/>
+      <c r="N34" s="92"/>
+      <c r="O34" s="92"/>
+      <c r="P34" s="92"/>
+      <c r="Q34" s="92"/>
+      <c r="R34" s="92"/>
+      <c r="S34" s="92"/>
+      <c r="T34" s="92"/>
+      <c r="U34" s="92"/>
+      <c r="V34" s="92"/>
+      <c r="W34" s="92"/>
+      <c r="X34" s="92"/>
+      <c r="Y34" s="92"/>
+      <c r="Z34" s="92"/>
+      <c r="AA34" s="92"/>
+      <c r="AB34" s="92"/>
+      <c r="AC34" s="92"/>
+      <c r="AD34" s="92"/>
+      <c r="AE34" s="92"/>
+      <c r="AF34" s="92"/>
+      <c r="AG34" s="92"/>
+      <c r="AH34" s="92"/>
+      <c r="AI34" s="92"/>
+      <c r="AJ34" s="93"/>
     </row>
     <row r="35" spans="1:36" ht="15" customHeight="1">
-      <c r="A35" s="92" t="s">
+      <c r="A35" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="92"/>
-      <c r="C35" s="92"/>
-      <c r="D35" s="92"/>
-      <c r="E35" s="92"/>
-      <c r="F35" s="92"/>
-      <c r="G35" s="92"/>
-      <c r="H35" s="92"/>
-      <c r="I35" s="92"/>
-      <c r="J35" s="92"/>
-      <c r="K35" s="92"/>
-      <c r="L35" s="92"/>
-      <c r="M35" s="92"/>
-      <c r="N35" s="92"/>
-      <c r="O35" s="92"/>
-      <c r="P35" s="92"/>
-      <c r="Q35" s="92"/>
-      <c r="R35" s="92"/>
-      <c r="S35" s="92"/>
-      <c r="T35" s="92"/>
-      <c r="U35" s="92"/>
-      <c r="V35" s="92"/>
-      <c r="W35" s="92"/>
-      <c r="X35" s="92"/>
-      <c r="Y35" s="92"/>
-      <c r="Z35" s="92"/>
-      <c r="AA35" s="92"/>
-      <c r="AB35" s="92"/>
-      <c r="AC35" s="92"/>
-      <c r="AD35" s="92"/>
-      <c r="AE35" s="92"/>
-      <c r="AF35" s="92"/>
-      <c r="AG35" s="92"/>
-      <c r="AH35" s="92"/>
-      <c r="AI35" s="92"/>
-      <c r="AJ35" s="92"/>
+      <c r="B35" s="83"/>
+      <c r="C35" s="83"/>
+      <c r="D35" s="83"/>
+      <c r="E35" s="83"/>
+      <c r="F35" s="83"/>
+      <c r="G35" s="83"/>
+      <c r="H35" s="83"/>
+      <c r="I35" s="83"/>
+      <c r="J35" s="83"/>
+      <c r="K35" s="83"/>
+      <c r="L35" s="83"/>
+      <c r="M35" s="83"/>
+      <c r="N35" s="83"/>
+      <c r="O35" s="83"/>
+      <c r="P35" s="83"/>
+      <c r="Q35" s="83"/>
+      <c r="R35" s="83"/>
+      <c r="S35" s="83"/>
+      <c r="T35" s="83"/>
+      <c r="U35" s="83"/>
+      <c r="V35" s="83"/>
+      <c r="W35" s="83"/>
+      <c r="X35" s="83"/>
+      <c r="Y35" s="83"/>
+      <c r="Z35" s="83"/>
+      <c r="AA35" s="83"/>
+      <c r="AB35" s="83"/>
+      <c r="AC35" s="83"/>
+      <c r="AD35" s="83"/>
+      <c r="AE35" s="83"/>
+      <c r="AF35" s="83"/>
+      <c r="AG35" s="83"/>
+      <c r="AH35" s="83"/>
+      <c r="AI35" s="83"/>
+      <c r="AJ35" s="83"/>
     </row>
     <row r="36" spans="1:36">
-      <c r="A36" s="93"/>
-      <c r="B36" s="93"/>
-      <c r="C36" s="93"/>
-      <c r="D36" s="93"/>
-      <c r="E36" s="93"/>
-      <c r="F36" s="93"/>
-      <c r="G36" s="93"/>
-      <c r="H36" s="93"/>
-      <c r="I36" s="93"/>
-      <c r="J36" s="93"/>
-      <c r="K36" s="93"/>
-      <c r="L36" s="93"/>
-      <c r="M36" s="93"/>
-      <c r="N36" s="93"/>
-      <c r="O36" s="93"/>
-      <c r="P36" s="93"/>
-      <c r="Q36" s="93"/>
-      <c r="R36" s="93"/>
-      <c r="S36" s="93"/>
-      <c r="T36" s="93"/>
-      <c r="U36" s="93"/>
-      <c r="V36" s="93"/>
-      <c r="W36" s="93"/>
-      <c r="X36" s="93"/>
-      <c r="Y36" s="93"/>
-      <c r="Z36" s="93"/>
-      <c r="AA36" s="93"/>
-      <c r="AB36" s="93"/>
-      <c r="AC36" s="93"/>
-      <c r="AD36" s="93"/>
-      <c r="AE36" s="93"/>
-      <c r="AF36" s="93"/>
-      <c r="AG36" s="93"/>
-      <c r="AH36" s="93"/>
-      <c r="AI36" s="93"/>
-      <c r="AJ36" s="93"/>
+      <c r="A36" s="84"/>
+      <c r="B36" s="84"/>
+      <c r="C36" s="84"/>
+      <c r="D36" s="84"/>
+      <c r="E36" s="84"/>
+      <c r="F36" s="84"/>
+      <c r="G36" s="84"/>
+      <c r="H36" s="84"/>
+      <c r="I36" s="84"/>
+      <c r="J36" s="84"/>
+      <c r="K36" s="84"/>
+      <c r="L36" s="84"/>
+      <c r="M36" s="84"/>
+      <c r="N36" s="84"/>
+      <c r="O36" s="84"/>
+      <c r="P36" s="84"/>
+      <c r="Q36" s="84"/>
+      <c r="R36" s="84"/>
+      <c r="S36" s="84"/>
+      <c r="T36" s="84"/>
+      <c r="U36" s="84"/>
+      <c r="V36" s="84"/>
+      <c r="W36" s="84"/>
+      <c r="X36" s="84"/>
+      <c r="Y36" s="84"/>
+      <c r="Z36" s="84"/>
+      <c r="AA36" s="84"/>
+      <c r="AB36" s="84"/>
+      <c r="AC36" s="84"/>
+      <c r="AD36" s="84"/>
+      <c r="AE36" s="84"/>
+      <c r="AF36" s="84"/>
+      <c r="AG36" s="84"/>
+      <c r="AH36" s="84"/>
+      <c r="AI36" s="84"/>
+      <c r="AJ36" s="84"/>
     </row>
     <row r="37" spans="1:36">
-      <c r="A37" s="93"/>
-      <c r="B37" s="93"/>
-      <c r="C37" s="93"/>
-      <c r="D37" s="93"/>
-      <c r="E37" s="93"/>
-      <c r="F37" s="93"/>
-      <c r="G37" s="93"/>
-      <c r="H37" s="93"/>
-      <c r="I37" s="93"/>
-      <c r="J37" s="93"/>
-      <c r="K37" s="93"/>
-      <c r="L37" s="93"/>
-      <c r="M37" s="93"/>
-      <c r="N37" s="93"/>
-      <c r="O37" s="93"/>
-      <c r="P37" s="93"/>
-      <c r="Q37" s="93"/>
-      <c r="R37" s="93"/>
-      <c r="S37" s="93"/>
-      <c r="T37" s="93"/>
-      <c r="U37" s="93"/>
-      <c r="V37" s="93"/>
-      <c r="W37" s="93"/>
-      <c r="X37" s="93"/>
-      <c r="Y37" s="93"/>
-      <c r="Z37" s="93"/>
-      <c r="AA37" s="93"/>
-      <c r="AB37" s="93"/>
-      <c r="AC37" s="93"/>
-      <c r="AD37" s="93"/>
-      <c r="AE37" s="93"/>
-      <c r="AF37" s="93"/>
-      <c r="AG37" s="93"/>
-      <c r="AH37" s="93"/>
-      <c r="AI37" s="93"/>
-      <c r="AJ37" s="93"/>
+      <c r="A37" s="84"/>
+      <c r="B37" s="84"/>
+      <c r="C37" s="84"/>
+      <c r="D37" s="84"/>
+      <c r="E37" s="84"/>
+      <c r="F37" s="84"/>
+      <c r="G37" s="84"/>
+      <c r="H37" s="84"/>
+      <c r="I37" s="84"/>
+      <c r="J37" s="84"/>
+      <c r="K37" s="84"/>
+      <c r="L37" s="84"/>
+      <c r="M37" s="84"/>
+      <c r="N37" s="84"/>
+      <c r="O37" s="84"/>
+      <c r="P37" s="84"/>
+      <c r="Q37" s="84"/>
+      <c r="R37" s="84"/>
+      <c r="S37" s="84"/>
+      <c r="T37" s="84"/>
+      <c r="U37" s="84"/>
+      <c r="V37" s="84"/>
+      <c r="W37" s="84"/>
+      <c r="X37" s="84"/>
+      <c r="Y37" s="84"/>
+      <c r="Z37" s="84"/>
+      <c r="AA37" s="84"/>
+      <c r="AB37" s="84"/>
+      <c r="AC37" s="84"/>
+      <c r="AD37" s="84"/>
+      <c r="AE37" s="84"/>
+      <c r="AF37" s="84"/>
+      <c r="AG37" s="84"/>
+      <c r="AH37" s="84"/>
+      <c r="AI37" s="84"/>
+      <c r="AJ37" s="84"/>
     </row>
     <row r="38" spans="1:36">
       <c r="O38" s="7"/>
@@ -9304,40 +9304,40 @@
       <c r="O39" s="22"/>
     </row>
     <row r="40" spans="1:36">
-      <c r="A40" s="91" t="s">
+      <c r="A40" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="91"/>
-      <c r="C40" s="91"/>
-      <c r="D40" s="91"/>
-      <c r="E40" s="91"/>
-      <c r="F40" s="91"/>
-      <c r="G40" s="91"/>
-      <c r="H40" s="91"/>
-      <c r="I40" s="91"/>
-      <c r="J40" s="91"/>
-      <c r="K40" s="91"/>
-      <c r="L40" s="91"/>
-      <c r="M40" s="91"/>
-      <c r="N40" s="91"/>
+      <c r="B40" s="82"/>
+      <c r="C40" s="82"/>
+      <c r="D40" s="82"/>
+      <c r="E40" s="82"/>
+      <c r="F40" s="82"/>
+      <c r="G40" s="82"/>
+      <c r="H40" s="82"/>
+      <c r="I40" s="82"/>
+      <c r="J40" s="82"/>
+      <c r="K40" s="82"/>
+      <c r="L40" s="82"/>
+      <c r="M40" s="82"/>
+      <c r="N40" s="82"/>
     </row>
     <row r="41" spans="1:36">
-      <c r="A41" s="90" t="s">
+      <c r="A41" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="90"/>
-      <c r="C41" s="90"/>
-      <c r="D41" s="90"/>
-      <c r="E41" s="90"/>
-      <c r="F41" s="90"/>
-      <c r="G41" s="90"/>
-      <c r="H41" s="90"/>
-      <c r="I41" s="90"/>
-      <c r="J41" s="90"/>
-      <c r="K41" s="90"/>
-      <c r="L41" s="90"/>
-      <c r="M41" s="90"/>
-      <c r="N41" s="90"/>
+      <c r="B41" s="81"/>
+      <c r="C41" s="81"/>
+      <c r="D41" s="81"/>
+      <c r="E41" s="81"/>
+      <c r="F41" s="81"/>
+      <c r="G41" s="81"/>
+      <c r="H41" s="81"/>
+      <c r="I41" s="81"/>
+      <c r="J41" s="81"/>
+      <c r="K41" s="81"/>
+      <c r="L41" s="81"/>
+      <c r="M41" s="81"/>
+      <c r="N41" s="81"/>
     </row>
     <row r="42" spans="1:36">
       <c r="A42" t="s">
@@ -9351,6 +9351,36 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="AE33:AF33"/>
+    <mergeCell ref="AH33:AJ33"/>
+    <mergeCell ref="A34:AJ34"/>
+    <mergeCell ref="AE25:AF25"/>
+    <mergeCell ref="AH25:AJ25"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="P33:Q33"/>
+    <mergeCell ref="S33:U33"/>
+    <mergeCell ref="W33:Y33"/>
+    <mergeCell ref="AA33:AC33"/>
+    <mergeCell ref="AA25:AC25"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="A1:AJ1"/>
+    <mergeCell ref="AA2:AJ2"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="S11:U11"/>
+    <mergeCell ref="W11:Y11"/>
+    <mergeCell ref="AA11:AC11"/>
+    <mergeCell ref="AE11:AF11"/>
+    <mergeCell ref="AH11:AJ11"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="S18:U18"/>
     <mergeCell ref="A41:N41"/>
@@ -9367,36 +9397,6 @@
     <mergeCell ref="P25:Q25"/>
     <mergeCell ref="S25:U25"/>
     <mergeCell ref="W25:Y25"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="A1:AJ1"/>
-    <mergeCell ref="AA2:AJ2"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="S11:U11"/>
-    <mergeCell ref="W11:Y11"/>
-    <mergeCell ref="AA11:AC11"/>
-    <mergeCell ref="AE11:AF11"/>
-    <mergeCell ref="AH11:AJ11"/>
-    <mergeCell ref="AE33:AF33"/>
-    <mergeCell ref="AH33:AJ33"/>
-    <mergeCell ref="A34:AJ34"/>
-    <mergeCell ref="AE25:AF25"/>
-    <mergeCell ref="AH25:AJ25"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="P33:Q33"/>
-    <mergeCell ref="S33:U33"/>
-    <mergeCell ref="W33:Y33"/>
-    <mergeCell ref="AA33:AC33"/>
-    <mergeCell ref="AA25:AC25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AL6" r:id="rId1"/>
@@ -9442,26 +9442,26 @@
   <sheetData>
     <row r="1" spans="1:21" ht="35.25">
       <c r="A1" s="29"/>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="106" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
-      <c r="O1" s="94"/>
-      <c r="P1" s="94"/>
-      <c r="Q1" s="94"/>
-      <c r="R1" s="94"/>
-      <c r="S1" s="94"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="106"/>
+      <c r="J1" s="106"/>
+      <c r="K1" s="106"/>
+      <c r="L1" s="106"/>
+      <c r="M1" s="106"/>
+      <c r="N1" s="106"/>
+      <c r="O1" s="106"/>
+      <c r="P1" s="106"/>
+      <c r="Q1" s="106"/>
+      <c r="R1" s="106"/>
+      <c r="S1" s="106"/>
       <c r="T1" s="68"/>
       <c r="U1" s="69"/>
     </row>
@@ -9481,47 +9481,47 @@
       <c r="M2" s="38"/>
       <c r="N2" s="72"/>
       <c r="O2" s="38"/>
-      <c r="P2" s="95" t="s">
+      <c r="P2" s="107" t="s">
         <v>243</v>
       </c>
-      <c r="Q2" s="95"/>
-      <c r="R2" s="95"/>
-      <c r="S2" s="95"/>
+      <c r="Q2" s="107"/>
+      <c r="R2" s="107"/>
+      <c r="S2" s="107"/>
       <c r="T2" s="38"/>
       <c r="U2" s="44"/>
     </row>
     <row r="3" spans="1:21" ht="18.75">
       <c r="A3" s="31"/>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="99" t="s">
+      <c r="C3" s="109"/>
+      <c r="D3" s="110"/>
+      <c r="E3" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="97"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="99" t="s">
+      <c r="F3" s="109"/>
+      <c r="G3" s="110"/>
+      <c r="H3" s="111" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="97"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="99" t="s">
+      <c r="I3" s="109"/>
+      <c r="J3" s="110"/>
+      <c r="K3" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="97"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="99" t="s">
+      <c r="L3" s="109"/>
+      <c r="M3" s="110"/>
+      <c r="N3" s="111" t="s">
         <v>40</v>
       </c>
-      <c r="O3" s="97"/>
-      <c r="P3" s="98"/>
-      <c r="Q3" s="99" t="s">
+      <c r="O3" s="109"/>
+      <c r="P3" s="110"/>
+      <c r="Q3" s="111" t="s">
         <v>41</v>
       </c>
-      <c r="R3" s="97"/>
-      <c r="S3" s="100"/>
+      <c r="R3" s="109"/>
+      <c r="S3" s="112"/>
       <c r="T3" s="38"/>
       <c r="U3" s="44"/>
     </row>
@@ -9597,36 +9597,36 @@
     </row>
     <row r="6" spans="1:21" ht="19.5" thickBot="1">
       <c r="A6" s="31"/>
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="100" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="107"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="106" t="s">
+      <c r="C6" s="95"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="107"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="106" t="s">
+      <c r="F6" s="95"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="94" t="s">
         <v>56</v>
       </c>
-      <c r="I6" s="107"/>
-      <c r="J6" s="108"/>
-      <c r="K6" s="106" t="s">
+      <c r="I6" s="95"/>
+      <c r="J6" s="96"/>
+      <c r="K6" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="L6" s="107"/>
-      <c r="M6" s="108"/>
-      <c r="N6" s="106" t="s">
+      <c r="L6" s="95"/>
+      <c r="M6" s="96"/>
+      <c r="N6" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="O6" s="107"/>
-      <c r="P6" s="108"/>
-      <c r="Q6" s="106" t="s">
+      <c r="O6" s="95"/>
+      <c r="P6" s="96"/>
+      <c r="Q6" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="R6" s="107"/>
-      <c r="S6" s="109"/>
+      <c r="R6" s="95"/>
+      <c r="S6" s="97"/>
       <c r="T6" s="38"/>
       <c r="U6" s="44"/>
     </row>
@@ -11402,26 +11402,26 @@
     </row>
     <row r="37" spans="1:21" ht="18.75">
       <c r="A37" s="31"/>
-      <c r="B37" s="111" t="s">
+      <c r="B37" s="99" t="s">
         <v>241</v>
       </c>
-      <c r="C37" s="111"/>
-      <c r="D37" s="111"/>
-      <c r="E37" s="111"/>
-      <c r="F37" s="111"/>
-      <c r="G37" s="111"/>
-      <c r="H37" s="111"/>
-      <c r="I37" s="111"/>
-      <c r="J37" s="111"/>
-      <c r="K37" s="111"/>
-      <c r="L37" s="111"/>
-      <c r="M37" s="111"/>
-      <c r="N37" s="111"/>
-      <c r="O37" s="111"/>
-      <c r="P37" s="111"/>
-      <c r="Q37" s="111"/>
-      <c r="R37" s="111"/>
-      <c r="S37" s="111"/>
+      <c r="C37" s="99"/>
+      <c r="D37" s="99"/>
+      <c r="E37" s="99"/>
+      <c r="F37" s="99"/>
+      <c r="G37" s="99"/>
+      <c r="H37" s="99"/>
+      <c r="I37" s="99"/>
+      <c r="J37" s="99"/>
+      <c r="K37" s="99"/>
+      <c r="L37" s="99"/>
+      <c r="M37" s="99"/>
+      <c r="N37" s="99"/>
+      <c r="O37" s="99"/>
+      <c r="P37" s="99"/>
+      <c r="Q37" s="99"/>
+      <c r="R37" s="99"/>
+      <c r="S37" s="99"/>
       <c r="T37" s="38"/>
       <c r="U37" s="44"/>
     </row>
@@ -11450,26 +11450,26 @@
     </row>
     <row r="39" spans="1:21">
       <c r="A39" s="31"/>
-      <c r="B39" s="110" t="s">
+      <c r="B39" s="98" t="s">
         <v>244</v>
       </c>
-      <c r="C39" s="110"/>
-      <c r="D39" s="110"/>
-      <c r="E39" s="110"/>
-      <c r="F39" s="110"/>
-      <c r="G39" s="110"/>
-      <c r="H39" s="110"/>
-      <c r="I39" s="110"/>
-      <c r="J39" s="110"/>
-      <c r="K39" s="110"/>
-      <c r="L39" s="110"/>
-      <c r="M39" s="110"/>
-      <c r="N39" s="110"/>
-      <c r="O39" s="110"/>
-      <c r="P39" s="110"/>
-      <c r="Q39" s="110"/>
-      <c r="R39" s="110"/>
-      <c r="S39" s="110"/>
+      <c r="C39" s="98"/>
+      <c r="D39" s="98"/>
+      <c r="E39" s="98"/>
+      <c r="F39" s="98"/>
+      <c r="G39" s="98"/>
+      <c r="H39" s="98"/>
+      <c r="I39" s="98"/>
+      <c r="J39" s="98"/>
+      <c r="K39" s="98"/>
+      <c r="L39" s="98"/>
+      <c r="M39" s="98"/>
+      <c r="N39" s="98"/>
+      <c r="O39" s="98"/>
+      <c r="P39" s="98"/>
+      <c r="Q39" s="98"/>
+      <c r="R39" s="98"/>
+      <c r="S39" s="98"/>
       <c r="T39" s="38"/>
       <c r="U39" s="44"/>
     </row>
@@ -11636,14 +11636,14 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="B39:S39"/>
-    <mergeCell ref="B37:S37"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="B1:S1"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
     <mergeCell ref="Q5:S5"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="E4:G4"/>
@@ -11656,14 +11656,14 @@
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="K5:M5"/>
     <mergeCell ref="N5:P5"/>
-    <mergeCell ref="B1:S1"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="B39:S39"/>
+    <mergeCell ref="B37:S37"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>